<commit_message>
IP address changed for source code api, proxy
</commit_message>
<xml_diff>
--- a/Group Mapping.xlsx
+++ b/Group Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Martin/code/cmu/azfour/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\AZFour5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A188A6-F345-E142-AEC5-E161C43AE203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641C5D78-5D66-4EE8-99F8-BBC317B29AF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="1300" windowWidth="28040" windowHeight="17440" xr2:uid="{98920742-2649-DF42-A49D-6FB5F4448CE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98920742-2649-DF42-A49D-6FB5F4448CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -449,23 +449,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E81D5CA-B0F8-384B-BE31-3F187DF8CBA3}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
-    <col min="10" max="10" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
+    <col min="7" max="7" width="18.625" customWidth="1"/>
+    <col min="8" max="8" width="17.625" customWidth="1"/>
+    <col min="9" max="9" width="22.625" customWidth="1"/>
+    <col min="10" max="10" width="25.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20">
+    <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -481,7 +484,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="20">
+    <row r="2" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -493,7 +496,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="20">
+    <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="20">
+    <row r="4" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -549,7 +552,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="20">
+    <row r="5" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -577,7 +580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="20">
+    <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -605,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="20">
+    <row r="7" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -633,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="20">
+    <row r="8" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -661,7 +664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="20">
+    <row r="9" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -689,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="20">
+    <row r="10" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -717,7 +720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="20">
+    <row r="13" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -741,5 +744,6 @@
     <mergeCell ref="G1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Survey updates, mapping fixed for orientations
</commit_message>
<xml_diff>
--- a/Group Mapping.xlsx
+++ b/Group Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronc\AZFour7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87F6BAE-72BF-4B88-8D1C-88CD3015428D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BF581A-7C09-46FD-BC2D-CA1EF5C44C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="885" windowWidth="24870" windowHeight="13740" activeTab="1" xr2:uid="{98920742-2649-DF42-A49D-6FB5F4448CE8}"/>
+    <workbookView xWindow="540" yWindow="2355" windowWidth="24120" windowHeight="14835" xr2:uid="{98920742-2649-DF42-A49D-6FB5F4448CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Group</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Play first</t>
   </si>
   <si>
-    <t>Receive Recom. First</t>
-  </si>
-  <si>
     <t>Opponent Level</t>
   </si>
   <si>
@@ -66,18 +63,9 @@
     <t>Recommender Display</t>
   </si>
   <si>
-    <t>Skill 4</t>
-  </si>
-  <si>
     <t>Oracle Level</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Low-High-Low</t>
   </si>
   <si>
@@ -87,9 +75,6 @@
     <t>High-Low-High</t>
   </si>
   <si>
-    <t>Experiment 2 Group Mapping (2x2x2)</t>
-  </si>
-  <si>
     <t>Oracle scaling for modified scoring</t>
   </si>
   <si>
@@ -178,6 +163,24 @@
   </si>
   <si>
     <t>ensure auth, auth2 are synchronized</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>display</t>
+  </si>
+  <si>
+    <t>Skill 5</t>
+  </si>
+  <si>
+    <t>Gen50</t>
+  </si>
+  <si>
+    <t>Skill 3</t>
+  </si>
+  <si>
+    <t>Experiment 2 Group Mapping (2x2)</t>
   </si>
 </sst>
 </file>
@@ -255,13 +258,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,10 +582,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -594,181 +597,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D7">
+    <sortCondition ref="A4:A7"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:D2"/>
   </mergeCells>
@@ -781,166 +731,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7702A2-15FA-44B5-903D-BFB3C6A9D60B}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="5"/>
+    <col min="1" max="1" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>34</v>
+      <c r="A1" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
+      <c r="A2" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>19</v>
+      <c r="A6" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
+      <c r="A10" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>21</v>
+      <c r="A14" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>22</v>
+      <c r="A18" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7"/>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>23</v>
+      <c r="A26" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>42</v>
+      <c r="A31" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>37</v>
+      <c r="A34" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>